<commit_message>
Added more comments to app.py & made few changes in code
</commit_message>
<xml_diff>
--- a/MegaACD Chatbot(3).xlsx
+++ b/MegaACD Chatbot(3).xlsx
@@ -188,43 +188,7 @@
     <t>What is a chatbot?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-A chatbot is a software application used to conduct an on-line chat conversation via text or text-to-speech, in lieu of providing direct contact with a live human agent. 
-</t>
-  </si>
-  <si>
-    <t>What features are planned to be available in the chatbot in the future?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A web interface has been provided on which data (in Excel files) can be uploaded. Once the upload is complete, chatbot will pick up the file and begin the training process.
-</t>
-  </si>
-  <si>
     <t>Input</t>
-  </si>
-  <si>
-    <t>What will happen if chatbot is asked a question that it does not understand but was trained on related question?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-When the chatbot trains, it reads through all the questions provided in the data, identifies keywords and looks up their synonyms. It then uses the frequency of the key words in the questions and their synonyms to associate them to responses provided in data. This enables chatbot to understand questions that asked are differently from the data questions and respond to them.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-It is possible that the chatbot is asked a question that it does not undertand even though it was trained on a question that was worded/phrased differently but had the same meaning. In this case it will respond by saying "Sorry, I do not understad the question. Can you please try saying it a different way?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-In this case the chatbot will respond by saying "Sorry, I do not understad the question. Can you please try saying it a different way?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A web interface has been provided where data (all possible questions and answers in an Excel file) can be uploaded easily for the chatbot to consume. 
-</t>
   </si>
   <si>
     <t>Does Mega offer a chatbot?</t>
@@ -244,12 +208,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Mega chatbot uses neural network and probability algorithm to identify the intent of the user input and present the most accurate response based on the data provided.
-When the chabot is provided data with any number of questions and their corresponding responses, it trains itself to learn all the questions and their responses. Once training is complete, when a user asks the chatbot a question, chatbot will identify the intent of the question asked by comparing it to the questions it was trained on using keywords and provide the most appropriate response.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mega chatbot's current limitations are:
 - It is not self-learning and data has to be provided manually via a web interface
 - It can only respond to questions that have been provided in the data 
@@ -258,31 +216,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Mega chatbot will not be a "chatty" bot and will not respond to customer inputs that are not related to a company's business, services, or products. 
-</t>
-  </si>
-  <si>
     <t>Using neural network and deep learning will enable Mega chatbot to understand the intent of user's input and the context of the conversation. This will enable the chatbot to:
 1) Respond to questions correctly even when asked differently from the questions in data provided
 2) Understand follow up  questions users may ask in reply to chatbot's response</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Mega chatbot will have the following features:
-- Use neural network and deep learning to understand the context of customers' queries in addition to the intent
-- Ability to access customer data through CRM and billing systems after customers log in, to identify products used and customers' history with the company
-- Provide customer an option (through a graphical button or text input) to speak to a human agent at any point in the chat
-- Ability to monitor real-time chat between human agents and customers and use the chat as data to train itself and enhance its capability to better interact with customers
-- Calculate the probability of being able to respond accurately and appropritely to all user inputs and only respond if probability is high. A low probability calculation will lead to customer being connected to an agent. This feature will help maintain good customer experience when using chatbot
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Through access to customer data through CRM and billing systems, products used by customers and their history with a company can be identified.  This will help better understand the context of customers' queries and provide support specific to individual customers based on their needs. 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mega is currently developing a chatbot as part of MegaACD. 
 </t>
   </si>
@@ -298,11 +236,6 @@
     <t>How will the chabot know how to respond to questions asked?
 How chatbot knows answers
 How chatbot respond</t>
-  </si>
-  <si>
-    <t>What happens during the training process?
-Training process
-how chatbot is trained</t>
   </si>
   <si>
     <t>How will the chatbot be trained?
@@ -314,10 +247,6 @@
   <si>
     <t>What is out of scope for the chatbot?
 Chatbot out of scope</t>
-  </si>
-  <si>
-    <t>What is the benefit or  purpose of allowing Mega chatbot to access customer data?
-Benefit Mega customer data</t>
   </si>
   <si>
     <t>What is the benefit or  purpose of using neural network and deep learning in Mega chatbot?
@@ -342,6 +271,71 @@
 Mega chatbot detail
 more about mega chatbot
 details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A chatbot is a software application used to conduct an on-line chat conversation via text or text-to-speech, in lieu of providing direct contact with a live human agent. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A web interface has been provided where data (all possible questions and answers in an Excel file) can be uploaded easily for the chatbot to consume. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega chatbot uses neural network and probability algorithm to identify the intent of the user input and present the most accurate response based on the data provided.
+When the chabot is provided data with any number of questions and their corresponding responses, it trains itself to learn all the questions and their responses. Once training is complete, when a user asks the chatbot a question, chatbot will identify the intent of the question asked by comparing it to the questions it was trained on using keywords and provide the most appropriate response.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A web interface has been provided on which data (in Excel files) can be uploaded. Once the upload is complete, chatbot will pick up the file and begin the training process.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the chatbot trains, it reads through all the questions provided in the data, identifies keywords and looks up their synonyms. It then uses the frequency of the key words in the questions and their synonyms to associate them to responses provided in data. This enables chatbot to understand questions that asked are differently from the data questions and respond to them.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this case the chatbot will respond by saying "Sorry, I do not understad the question. Can you please try saying it a different way?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega chatbot will have the following features:
+- Use neural network and deep learning to understand the context of customers' queries in addition to the intent
+- Ability to access customer data through CRM and billing systems after customers log in, to identify products used and customers' history with the company
+- Provide customer an option (through a graphical button or text input) to speak to a human agent at any point in the chat
+- Ability to monitor real-time chat between human agents and customers and use the chat as data to train itself and enhance its capability to better interact with customers
+- Calculate the probability of being able to respond accurately and appropritely to all user inputs and only respond if probability is high. A low probability calculation will lead to customer being connected to an agent. This feature will help maintain good customer experience when using chatbot
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mega chatbot will not be a "chatty" bot and will not respond to customer inputs that are not related to a company's business, services, or products. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through access to customer data through CRM and billing systems, products used by customers and their history with a company can be identified.  This will help better understand the context of customers' queries and provide support specific to individual customers based on their needs. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is possible that the chatbot is asked a question that it does not undertand even though it was trained on a question that was worded/phrased differently but had the same meaning. In this case it will respond by saying "Sorry, I do not understad the question. Can you please try saying it a different way?
+</t>
+  </si>
+  <si>
+    <t>What happens during the training process?
+Training process
+how chatbot is trained
+how chatbot learn</t>
+  </si>
+  <si>
+    <t>What will happen if chatbot is asked a question that it does not understand but was trained on related question?
+Unrelated question</t>
+  </si>
+  <si>
+    <t>What is the benefit or  purpose of allowing Mega chatbot to access customer data?
+why access customer data</t>
+  </si>
+  <si>
+    <t>What features are planned to be available in the chatbot in the future?
+Future features in our chatbot
+coming features in chatbot</t>
   </si>
 </sst>
 </file>
@@ -852,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>25</v>
@@ -874,124 +868,124 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="228.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="288" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>